<commit_message>
wroking on finding probs for each reward value, not there yet
</commit_message>
<xml_diff>
--- a/data/monetary/M_1011.xlsx
+++ b/data/monetary/M_1011.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-effort/data/monetary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E4DA55-7729-4F48-8C46-FF8B555D4415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02330AA-3546-014D-8959-D1368839AC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="1120" windowWidth="21580" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -964,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I68"/>
+    <sheetView tabSelected="1" topLeftCell="O61" workbookViewId="0">
+      <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8247,642 +8247,858 @@
       </c>
     </row>
     <row r="69" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69" t="s">
         <v>26</v>
       </c>
-      <c r="B69">
+      <c r="K69">
         <v>1011</v>
       </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="L69">
+        <v>1</v>
+      </c>
+      <c r="M69" t="s">
         <v>31</v>
       </c>
-      <c r="E69">
+      <c r="N69">
         <v>60.01</v>
       </c>
-      <c r="F69">
-        <v>1</v>
-      </c>
-      <c r="G69">
+      <c r="O69">
+        <v>1</v>
+      </c>
+      <c r="P69">
         <v>2105367534</v>
       </c>
-      <c r="H69" s="1">
+      <c r="Q69" s="1">
         <v>43878</v>
       </c>
-      <c r="I69" s="2">
+      <c r="R69" s="2">
         <v>43878.735671296294</v>
       </c>
-      <c r="J69" s="3">
+      <c r="S69" s="3">
         <v>0.52733796296296298</v>
       </c>
-      <c r="K69">
+      <c r="T69">
         <v>68</v>
       </c>
-      <c r="L69">
+      <c r="U69">
         <v>1.33</v>
       </c>
-      <c r="M69">
-        <v>1</v>
-      </c>
-      <c r="N69">
-        <v>1</v>
-      </c>
-      <c r="O69">
+      <c r="V69">
+        <v>1</v>
+      </c>
+      <c r="W69">
+        <v>1</v>
+      </c>
+      <c r="X69">
         <v>346</v>
       </c>
-      <c r="P69" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q69" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R69" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S69">
+      <c r="Y69" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z69" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA69" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB69">
         <v>50</v>
       </c>
-      <c r="T69" t="s">
+      <c r="AC69" t="s">
         <v>30</v>
       </c>
-      <c r="U69" t="s">
+      <c r="AD69" t="s">
         <v>22</v>
       </c>
-      <c r="V69">
+      <c r="AE69">
         <v>0.15798000000000001</v>
       </c>
-      <c r="W69">
+      <c r="AF69">
         <v>64</v>
       </c>
-      <c r="X69">
-        <v>1</v>
-      </c>
-      <c r="Y69">
+      <c r="AG69">
+        <v>1</v>
+      </c>
+      <c r="AH69">
         <v>64</v>
       </c>
-      <c r="Z69">
+      <c r="AI69">
         <v>1.33</v>
       </c>
     </row>
     <row r="70" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="A70">
+        <v>0</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70" t="s">
         <v>26</v>
       </c>
-      <c r="B70">
+      <c r="K70">
         <v>1011</v>
       </c>
-      <c r="C70">
-        <v>1</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="L70">
+        <v>1</v>
+      </c>
+      <c r="M70" t="s">
         <v>31</v>
       </c>
-      <c r="E70">
+      <c r="N70">
         <v>60.01</v>
       </c>
-      <c r="F70">
-        <v>1</v>
-      </c>
-      <c r="G70">
+      <c r="O70">
+        <v>1</v>
+      </c>
+      <c r="P70">
         <v>2105367534</v>
       </c>
-      <c r="H70" s="1">
+      <c r="Q70" s="1">
         <v>43878</v>
       </c>
-      <c r="I70" s="2">
+      <c r="R70" s="2">
         <v>43878.735671296294</v>
       </c>
-      <c r="J70" s="3">
+      <c r="S70" s="3">
         <v>0.52733796296296298</v>
       </c>
-      <c r="K70">
+      <c r="T70">
         <v>69</v>
       </c>
-      <c r="L70">
+      <c r="U70">
         <v>1.87</v>
       </c>
-      <c r="M70">
-        <v>1</v>
-      </c>
-      <c r="N70">
-        <v>1</v>
-      </c>
-      <c r="O70">
+      <c r="V70">
+        <v>1</v>
+      </c>
+      <c r="W70">
+        <v>1</v>
+      </c>
+      <c r="X70">
         <v>235</v>
       </c>
-      <c r="P70" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q70" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R70" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S70">
+      <c r="Y70" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z70" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA70" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB70">
         <v>50</v>
       </c>
-      <c r="T70" t="s">
+      <c r="AC70" t="s">
         <v>30</v>
       </c>
-      <c r="U70" t="s">
+      <c r="AD70" t="s">
         <v>22</v>
       </c>
-      <c r="V70">
+      <c r="AE70">
         <v>0.18414</v>
       </c>
-      <c r="W70">
+      <c r="AF70">
         <v>65</v>
       </c>
-      <c r="X70">
-        <v>1</v>
-      </c>
-      <c r="Y70">
+      <c r="AG70">
+        <v>1</v>
+      </c>
+      <c r="AH70">
         <v>65</v>
       </c>
-      <c r="Z70">
+      <c r="AI70">
         <v>1.87</v>
       </c>
     </row>
     <row r="71" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="A71">
+        <v>0</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71" t="s">
         <v>26</v>
       </c>
-      <c r="B71">
+      <c r="K71">
         <v>1011</v>
       </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="L71">
+        <v>1</v>
+      </c>
+      <c r="M71" t="s">
         <v>31</v>
       </c>
-      <c r="E71">
+      <c r="N71">
         <v>60.01</v>
       </c>
-      <c r="F71">
-        <v>1</v>
-      </c>
-      <c r="G71">
+      <c r="O71">
+        <v>1</v>
+      </c>
+      <c r="P71">
         <v>2105367534</v>
       </c>
-      <c r="H71" s="1">
+      <c r="Q71" s="1">
         <v>43878</v>
       </c>
-      <c r="I71" s="2">
+      <c r="R71" s="2">
         <v>43878.735671296294</v>
       </c>
-      <c r="J71" s="3">
+      <c r="S71" s="3">
         <v>0.52733796296296298</v>
       </c>
-      <c r="K71">
+      <c r="T71">
         <v>70</v>
       </c>
-      <c r="L71">
+      <c r="U71">
         <v>1.51</v>
       </c>
-      <c r="M71">
-        <v>1</v>
-      </c>
-      <c r="N71">
-        <v>1</v>
-      </c>
-      <c r="O71">
+      <c r="V71">
+        <v>1</v>
+      </c>
+      <c r="W71">
+        <v>1</v>
+      </c>
+      <c r="X71">
         <v>96</v>
       </c>
-      <c r="P71" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q71" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R71" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S71">
+      <c r="Y71" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z71" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA71" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB71">
         <v>50</v>
       </c>
-      <c r="T71" t="s">
+      <c r="AC71" t="s">
         <v>30</v>
       </c>
-      <c r="U71" t="s">
+      <c r="AD71" t="s">
         <v>22</v>
       </c>
-      <c r="V71">
+      <c r="AE71">
         <v>0.17332</v>
       </c>
-      <c r="W71">
+      <c r="AF71">
         <v>66</v>
       </c>
-      <c r="X71">
-        <v>1</v>
-      </c>
-      <c r="Y71">
+      <c r="AG71">
+        <v>1</v>
+      </c>
+      <c r="AH71">
         <v>66</v>
       </c>
-      <c r="Z71">
+      <c r="AI71">
         <v>1.51</v>
       </c>
     </row>
     <row r="72" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72" t="s">
         <v>26</v>
       </c>
-      <c r="B72">
+      <c r="K72">
         <v>1011</v>
       </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="L72">
+        <v>1</v>
+      </c>
+      <c r="M72" t="s">
         <v>31</v>
       </c>
-      <c r="E72">
+      <c r="N72">
         <v>60.01</v>
       </c>
-      <c r="F72">
-        <v>1</v>
-      </c>
-      <c r="G72">
+      <c r="O72">
+        <v>1</v>
+      </c>
+      <c r="P72">
         <v>2105367534</v>
       </c>
-      <c r="H72" s="1">
+      <c r="Q72" s="1">
         <v>43878</v>
       </c>
-      <c r="I72" s="2">
+      <c r="R72" s="2">
         <v>43878.735671296294</v>
       </c>
-      <c r="J72" s="3">
+      <c r="S72" s="3">
         <v>0.52733796296296298</v>
       </c>
-      <c r="K72">
+      <c r="T72">
         <v>71</v>
       </c>
-      <c r="L72">
+      <c r="U72">
         <v>3.13</v>
       </c>
-      <c r="M72">
-        <v>0</v>
-      </c>
-      <c r="N72">
-        <v>1</v>
-      </c>
-      <c r="O72">
+      <c r="V72">
+        <v>0</v>
+      </c>
+      <c r="W72">
+        <v>1</v>
+      </c>
+      <c r="X72">
         <v>437</v>
       </c>
-      <c r="P72" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q72" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R72" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S72">
+      <c r="Y72" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z72" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA72" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB72">
         <v>88</v>
       </c>
-      <c r="T72" t="s">
+      <c r="AC72" t="s">
         <v>30</v>
       </c>
-      <c r="U72" t="s">
+      <c r="AD72" t="s">
         <v>22</v>
       </c>
-      <c r="V72">
+      <c r="AE72">
         <v>0.18723329999999999</v>
       </c>
-      <c r="W72">
+      <c r="AF72">
         <v>67</v>
       </c>
-      <c r="X72">
-        <v>1</v>
-      </c>
-      <c r="Y72">
+      <c r="AG72">
+        <v>1</v>
+      </c>
+      <c r="AH72">
         <v>67</v>
       </c>
-      <c r="Z72">
+      <c r="AI72">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="A73">
+        <v>0</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73" t="s">
         <v>26</v>
       </c>
-      <c r="B73">
+      <c r="K73">
         <v>1011</v>
       </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="L73">
+        <v>1</v>
+      </c>
+      <c r="M73" t="s">
         <v>31</v>
       </c>
-      <c r="E73">
+      <c r="N73">
         <v>60.01</v>
       </c>
-      <c r="F73">
-        <v>1</v>
-      </c>
-      <c r="G73">
+      <c r="O73">
+        <v>1</v>
+      </c>
+      <c r="P73">
         <v>2105367534</v>
       </c>
-      <c r="H73" s="1">
+      <c r="Q73" s="1">
         <v>43878</v>
       </c>
-      <c r="I73" s="2">
+      <c r="R73" s="2">
         <v>43878.735671296294</v>
       </c>
-      <c r="J73" s="3">
+      <c r="S73" s="3">
         <v>0.52733796296296298</v>
       </c>
-      <c r="K73">
+      <c r="T73">
         <v>72</v>
       </c>
-      <c r="L73">
+      <c r="U73">
         <v>3.13</v>
       </c>
-      <c r="M73">
-        <v>0</v>
-      </c>
-      <c r="N73">
-        <v>1</v>
-      </c>
-      <c r="O73">
+      <c r="V73">
+        <v>0</v>
+      </c>
+      <c r="W73">
+        <v>1</v>
+      </c>
+      <c r="X73">
         <v>160</v>
       </c>
-      <c r="P73" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q73" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R73" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S73">
+      <c r="Y73" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z73" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA73" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB73">
         <v>12</v>
       </c>
-      <c r="T73" t="s">
+      <c r="AC73" t="s">
         <v>29</v>
       </c>
-      <c r="U73" t="s">
+      <c r="AD73" t="s">
         <v>22</v>
       </c>
-      <c r="V73">
+      <c r="AE73">
         <v>0.1672333</v>
       </c>
-      <c r="W73">
+      <c r="AF73">
         <v>68</v>
       </c>
-      <c r="X73">
-        <v>1</v>
-      </c>
-      <c r="Y73">
+      <c r="AG73">
+        <v>1</v>
+      </c>
+      <c r="AH73">
         <v>68</v>
       </c>
-      <c r="Z73">
+      <c r="AI73">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="A74">
+        <v>0</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74" t="s">
         <v>26</v>
       </c>
-      <c r="B74">
+      <c r="K74">
         <v>1011</v>
       </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="L74">
+        <v>1</v>
+      </c>
+      <c r="M74" t="s">
         <v>31</v>
       </c>
-      <c r="E74">
+      <c r="N74">
         <v>60.01</v>
       </c>
-      <c r="F74">
-        <v>1</v>
-      </c>
-      <c r="G74">
+      <c r="O74">
+        <v>1</v>
+      </c>
+      <c r="P74">
         <v>2105367534</v>
       </c>
-      <c r="H74" s="1">
+      <c r="Q74" s="1">
         <v>43878</v>
       </c>
-      <c r="I74" s="2">
+      <c r="R74" s="2">
         <v>43878.735671296294</v>
       </c>
-      <c r="J74" s="3">
+      <c r="S74" s="3">
         <v>0.52733796296296298</v>
       </c>
-      <c r="K74">
+      <c r="T74">
         <v>73</v>
       </c>
-      <c r="L74">
+      <c r="U74">
         <v>3.85</v>
       </c>
-      <c r="M74">
-        <v>1</v>
-      </c>
-      <c r="N74">
-        <v>1</v>
-      </c>
-      <c r="O74">
+      <c r="V74">
+        <v>1</v>
+      </c>
+      <c r="W74">
+        <v>1</v>
+      </c>
+      <c r="X74">
         <v>245</v>
       </c>
-      <c r="P74" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q74" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R74" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S74">
+      <c r="Y74" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z74" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA74" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB74">
         <v>12</v>
       </c>
-      <c r="T74" t="s">
+      <c r="AC74" t="s">
         <v>29</v>
       </c>
-      <c r="U74" t="s">
+      <c r="AD74" t="s">
         <v>22</v>
       </c>
-      <c r="V74">
+      <c r="AE74">
         <v>0.16682</v>
       </c>
-      <c r="W74">
+      <c r="AF74">
         <v>69</v>
       </c>
-      <c r="X74">
-        <v>1</v>
-      </c>
-      <c r="Y74">
+      <c r="AG74">
+        <v>1</v>
+      </c>
+      <c r="AH74">
         <v>69</v>
       </c>
-      <c r="Z74">
+      <c r="AI74">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="A75">
+        <v>0</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75" t="s">
         <v>26</v>
       </c>
-      <c r="B75">
+      <c r="K75">
         <v>1011</v>
       </c>
-      <c r="C75">
-        <v>1</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="L75">
+        <v>1</v>
+      </c>
+      <c r="M75" t="s">
         <v>31</v>
       </c>
-      <c r="E75">
+      <c r="N75">
         <v>60.01</v>
       </c>
-      <c r="F75">
-        <v>1</v>
-      </c>
-      <c r="G75">
+      <c r="O75">
+        <v>1</v>
+      </c>
+      <c r="P75">
         <v>2105367534</v>
       </c>
-      <c r="H75" s="1">
+      <c r="Q75" s="1">
         <v>43878</v>
       </c>
-      <c r="I75" s="2">
+      <c r="R75" s="2">
         <v>43878.735671296294</v>
       </c>
-      <c r="J75" s="3">
+      <c r="S75" s="3">
         <v>0.52733796296296298</v>
       </c>
-      <c r="K75">
+      <c r="T75">
         <v>74</v>
       </c>
-      <c r="L75">
+      <c r="U75">
         <v>2.59</v>
       </c>
-      <c r="M75">
-        <v>0</v>
-      </c>
-      <c r="N75">
-        <v>1</v>
-      </c>
-      <c r="O75">
+      <c r="V75">
+        <v>0</v>
+      </c>
+      <c r="W75">
+        <v>1</v>
+      </c>
+      <c r="X75">
         <v>22</v>
       </c>
-      <c r="P75" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q75" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R75" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S75">
+      <c r="Y75" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z75" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA75" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB75">
         <v>88</v>
       </c>
-      <c r="T75" t="s">
+      <c r="AC75" t="s">
         <v>30</v>
       </c>
-      <c r="U75" t="s">
+      <c r="AD75" t="s">
         <v>22</v>
       </c>
-      <c r="V75">
+      <c r="AE75">
         <v>0.1594333</v>
       </c>
-      <c r="W75">
+      <c r="AF75">
         <v>70</v>
       </c>
-      <c r="X75">
-        <v>1</v>
-      </c>
-      <c r="Y75">
+      <c r="AG75">
+        <v>1</v>
+      </c>
+      <c r="AH75">
         <v>70</v>
       </c>
-      <c r="Z75">
+      <c r="AI75">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="A76">
+        <v>0</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76" t="s">
         <v>26</v>
       </c>
-      <c r="B76">
+      <c r="K76">
         <v>1011</v>
       </c>
-      <c r="C76">
-        <v>1</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="L76">
+        <v>1</v>
+      </c>
+      <c r="M76" t="s">
         <v>31</v>
       </c>
-      <c r="E76">
+      <c r="N76">
         <v>60.01</v>
       </c>
-      <c r="F76">
-        <v>1</v>
-      </c>
-      <c r="G76">
+      <c r="O76">
+        <v>1</v>
+      </c>
+      <c r="P76">
         <v>2105367534</v>
       </c>
-      <c r="H76" s="1">
+      <c r="Q76" s="1">
         <v>43878</v>
       </c>
-      <c r="I76" s="2">
+      <c r="R76" s="2">
         <v>43878.735671296294</v>
       </c>
-      <c r="J76" s="3">
+      <c r="S76" s="3">
         <v>0.52733796296296298</v>
       </c>
-      <c r="K76">
+      <c r="T76">
         <v>75</v>
       </c>
-      <c r="L76">
+      <c r="U76">
         <v>4.21</v>
       </c>
-      <c r="M76">
-        <v>1</v>
-      </c>
-      <c r="N76">
-        <v>1</v>
-      </c>
-      <c r="O76">
+      <c r="V76">
+        <v>1</v>
+      </c>
+      <c r="W76">
+        <v>1</v>
+      </c>
+      <c r="X76">
         <v>1579</v>
       </c>
-      <c r="P76" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q76" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R76" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S76">
+      <c r="Y76" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z76" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA76" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB76">
         <v>12</v>
       </c>
-      <c r="T76" t="s">
+      <c r="AC76" t="s">
         <v>29</v>
       </c>
-      <c r="U76" t="s">
+      <c r="AD76" t="s">
         <v>22</v>
       </c>
-      <c r="V76">
+      <c r="AE76">
         <v>0.15731000000000001</v>
       </c>
-      <c r="W76">
+      <c r="AF76">
         <v>71</v>
       </c>
-      <c r="X76">
-        <v>1</v>
-      </c>
-      <c r="Y76">
+      <c r="AG76">
+        <v>1</v>
+      </c>
+      <c r="AH76">
         <v>71</v>
       </c>
-      <c r="Z76">
+      <c r="AI76">
         <v>0</v>
       </c>
     </row>

</xml_diff>